<commit_message>
update sampel dan database
</commit_message>
<xml_diff>
--- a/sampel/Data Semester Tahun 2025.xlsx
+++ b/sampel/Data Semester Tahun 2025.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="5">
   <si>
     <t>Data Semester Tahun 2025</t>
   </si>
@@ -23,10 +23,13 @@
     <t>No</t>
   </si>
   <si>
-    <t>Id Semester</t>
+    <t>Tahun 1</t>
   </si>
   <si>
-    <t>Tahun</t>
+    <t>Tahun 2</t>
+  </si>
+  <si>
+    <t>Semester</t>
   </si>
 </sst>
 </file>
@@ -412,25 +415,26 @@
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:C5"/>
+  <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col min="1" max="1" width="3.427734" bestFit="true" customWidth="true" style="0"/>
-    <col min="2" max="2" width="13.996582" bestFit="true" customWidth="true" style="0"/>
-    <col min="3" max="3" width="6.998291" bestFit="true" customWidth="true" style="0"/>
+    <col min="2" max="2" width="9.283447" bestFit="true" customWidth="true" style="0"/>
+    <col min="3" max="3" width="9.283447" bestFit="true" customWidth="true" style="0"/>
+    <col min="4" max="4" width="10.568848" bestFit="true" customWidth="true" style="0"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:4">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:3">
+    <row r="3" spans="1:4">
       <c r="A3" s="2" t="s">
         <v>1</v>
       </c>
@@ -440,33 +444,42 @@
       <c r="C3" s="2" t="s">
         <v>3</v>
       </c>
+      <c r="D3" s="2" t="s">
+        <v>4</v>
+      </c>
     </row>
-    <row r="4" spans="1:3">
+    <row r="4" spans="1:4">
       <c r="A4" s="3">
         <v>1</v>
       </c>
       <c r="B4" s="3">
+        <v>2024</v>
+      </c>
+      <c r="C4" s="3">
+        <v>2025</v>
+      </c>
+      <c r="D4" s="3">
         <v>1</v>
       </c>
-      <c r="C4" s="3">
-        <v>2024</v>
-      </c>
     </row>
-    <row r="5" spans="1:3">
+    <row r="5" spans="1:4">
       <c r="A5" s="3">
         <v>2</v>
       </c>
       <c r="B5" s="3">
-        <v>2</v>
+        <v>2024</v>
       </c>
       <c r="C5" s="3">
         <v>2025</v>
+      </c>
+      <c r="D5" s="3">
+        <v>2</v>
       </c>
     </row>
   </sheetData>
   <sheetProtection sheet="false" objects="false" scenarios="false" formatCells="false" formatColumns="false" formatRows="false" insertColumns="false" insertRows="false" insertHyperlinks="false" deleteColumns="false" deleteRows="false" selectLockedCells="false" sort="false" autoFilter="false" pivotTables="false" selectUnlockedCells="false"/>
   <mergeCells>
-    <mergeCell ref="A1:C1"/>
+    <mergeCell ref="A1:D1"/>
   </mergeCells>
   <printOptions gridLines="false" gridLinesSet="true"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>